<commit_message>
last commit, work done
</commit_message>
<xml_diff>
--- a/auxiliar/casList.xlsx
+++ b/auxiliar/casList.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="487">
   <si>
     <t>CAS-number</t>
   </si>
@@ -332,9 +332,6 @@
     <t>oxirane, 2-methyl-, polymer with oxirane, monododecyl ether</t>
   </si>
   <si>
-    <t>ola</t>
-  </si>
-  <si>
     <t>(768)</t>
   </si>
   <si>
@@ -351,9 +348,6 @@
   </si>
   <si>
     <t>Sodium oleate</t>
-  </si>
-  <si>
-    <t>ga</t>
   </si>
   <si>
     <t>(686)</t>
@@ -2053,1555 +2047,1547 @@
       <c r="C36" t="s">
         <v>104</v>
       </c>
-      <c r="D36" t="s">
-        <v>105</v>
-      </c>
+      <c r="D36" s="2"/>
     </row>
     <row r="37">
       <c r="A37" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
         <v>106</v>
-      </c>
-      <c r="B37" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" t="s">
-        <v>107</v>
       </c>
       <c r="D37" s="2"/>
     </row>
     <row r="38">
       <c r="A38" t="s">
+        <v>107</v>
+      </c>
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
         <v>108</v>
-      </c>
-      <c r="B38" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" t="s">
-        <v>109</v>
       </c>
       <c r="D38" s="2"/>
     </row>
     <row r="39">
       <c r="A39" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
         <v>110</v>
       </c>
-      <c r="B39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" t="s">
-        <v>111</v>
-      </c>
-      <c r="D39" t="s">
-        <v>112</v>
-      </c>
+      <c r="D39" s="2"/>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B40" t="s">
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D40" s="2"/>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B41" t="s">
         <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D41" s="2"/>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B42" t="s">
         <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D42" s="2"/>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B43" t="s">
         <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>120</v>
-      </c>
-      <c r="D43" t="s">
-        <v>112</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="D43" s="2"/>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B44" t="s">
         <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D44" s="2"/>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B45" t="s">
         <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D45" s="2"/>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B46" t="s">
         <v>5</v>
       </c>
       <c r="C46" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D46" s="2"/>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B47" t="s">
         <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D47" s="2"/>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B48" t="s">
         <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D48" s="2"/>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B49" t="s">
         <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>132</v>
-      </c>
-      <c r="D49" t="s">
-        <v>112</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="D49" s="2"/>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B50" t="s">
         <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D50" s="2"/>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B51" t="s">
         <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D51" s="2"/>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B52" t="s">
         <v>5</v>
       </c>
       <c r="C52" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D52" s="2"/>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B53" t="s">
         <v>5</v>
       </c>
       <c r="C53" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D53" s="2"/>
     </row>
     <row r="54">
       <c r="A54" t="s">
+        <v>139</v>
+      </c>
+      <c r="B54" t="s">
+        <v>140</v>
+      </c>
+      <c r="C54" t="s">
         <v>141</v>
-      </c>
-      <c r="B54" t="s">
-        <v>142</v>
-      </c>
-      <c r="C54" t="s">
-        <v>143</v>
       </c>
       <c r="D54" s="2"/>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B55" t="s">
         <v>5</v>
       </c>
       <c r="C55" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D55" s="2"/>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B56" t="s">
         <v>5</v>
       </c>
       <c r="C56" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D56" s="2"/>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B57" t="s">
         <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D57" s="2"/>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B58" t="s">
         <v>5</v>
       </c>
       <c r="C58" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D58" s="2"/>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B59" t="s">
         <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D59" s="2"/>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B60" t="s">
         <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D60" s="2"/>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B61" t="s">
         <v>5</v>
       </c>
       <c r="C61" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D61" s="2"/>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B62" t="s">
         <v>5</v>
       </c>
       <c r="C62" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D62" s="2"/>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B63" t="s">
         <v>5</v>
       </c>
       <c r="C63" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D63" s="2"/>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B64" t="s">
         <v>5</v>
       </c>
       <c r="C64" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D64" s="2"/>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B65" t="s">
         <v>5</v>
       </c>
       <c r="C65" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D65" s="2"/>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B66" t="s">
         <v>5</v>
       </c>
       <c r="C66" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D66" s="2"/>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B67" t="s">
         <v>5</v>
       </c>
       <c r="C67" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D67" s="2"/>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B68" t="s">
         <v>5</v>
       </c>
       <c r="C68" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D68" s="2"/>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B69" t="s">
         <v>5</v>
       </c>
       <c r="C69" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D69" s="2"/>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B70" t="s">
         <v>5</v>
       </c>
       <c r="C70" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D70" s="2"/>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B71" t="s">
         <v>5</v>
       </c>
       <c r="C71" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D71" s="2"/>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B72" t="s">
         <v>5</v>
       </c>
       <c r="C72" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D72" s="2"/>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B73" t="s">
         <v>5</v>
       </c>
       <c r="C73" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D73" s="2"/>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B74" t="s">
         <v>5</v>
       </c>
       <c r="C74" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D74" s="2"/>
     </row>
     <row r="75">
       <c r="A75" t="s">
+        <v>182</v>
+      </c>
+      <c r="B75" t="s">
+        <v>183</v>
+      </c>
+      <c r="C75" t="s">
         <v>184</v>
-      </c>
-      <c r="B75" t="s">
-        <v>185</v>
-      </c>
-      <c r="C75" t="s">
-        <v>186</v>
       </c>
       <c r="D75" s="2"/>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B76" t="s">
         <v>5</v>
       </c>
       <c r="C76" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D76" s="2"/>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B77" t="s">
         <v>5</v>
       </c>
       <c r="C77" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D77" s="2"/>
     </row>
     <row r="78">
       <c r="A78" t="s">
+        <v>189</v>
+      </c>
+      <c r="B78" t="s">
+        <v>190</v>
+      </c>
+      <c r="C78" t="s">
         <v>191</v>
-      </c>
-      <c r="B78" t="s">
-        <v>192</v>
-      </c>
-      <c r="C78" t="s">
-        <v>193</v>
       </c>
       <c r="D78" s="2"/>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B79" t="s">
         <v>5</v>
       </c>
       <c r="C79" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D79" s="2"/>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B80" t="s">
         <v>5</v>
       </c>
       <c r="C80" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D80" s="2"/>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B81" t="s">
         <v>5</v>
       </c>
       <c r="C81" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D81" s="2"/>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B82" t="s">
         <v>5</v>
       </c>
       <c r="C82" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D82" s="2"/>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B83" t="s">
         <v>5</v>
       </c>
       <c r="C83" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D83" s="2"/>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B84" t="s">
         <v>5</v>
       </c>
       <c r="C84" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D84" s="2"/>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B85" t="s">
         <v>5</v>
       </c>
       <c r="C85" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D85" s="2"/>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B86" t="s">
         <v>5</v>
       </c>
       <c r="C86" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D86" s="2"/>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B87" t="s">
         <v>5</v>
       </c>
       <c r="C87" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D87" s="2"/>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B88" t="s">
         <v>5</v>
       </c>
       <c r="C88" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D88" s="2"/>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B89" t="s">
         <v>5</v>
       </c>
       <c r="C89" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D89" s="2"/>
     </row>
     <row r="90">
       <c r="A90" t="s">
+        <v>214</v>
+      </c>
+      <c r="B90" t="s">
+        <v>215</v>
+      </c>
+      <c r="C90" t="s">
         <v>216</v>
-      </c>
-      <c r="B90" t="s">
-        <v>217</v>
-      </c>
-      <c r="C90" t="s">
-        <v>218</v>
       </c>
       <c r="D90" s="2"/>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B91" t="s">
         <v>5</v>
       </c>
       <c r="C91" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D91" s="2"/>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B92" t="s">
         <v>5</v>
       </c>
       <c r="C92" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D92" s="2"/>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B93" t="s">
         <v>5</v>
       </c>
       <c r="C93" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D93" s="2"/>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B94" t="s">
         <v>5</v>
       </c>
       <c r="C94" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D94" s="2"/>
     </row>
     <row r="95">
       <c r="A95" t="s">
+        <v>225</v>
+      </c>
+      <c r="B95" t="s">
+        <v>226</v>
+      </c>
+      <c r="C95" t="s">
         <v>227</v>
-      </c>
-      <c r="B95" t="s">
-        <v>228</v>
-      </c>
-      <c r="C95" t="s">
-        <v>229</v>
       </c>
       <c r="D95" s="2"/>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B96" t="s">
         <v>5</v>
       </c>
       <c r="C96" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D96" s="2"/>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B97" t="s">
         <v>5</v>
       </c>
       <c r="C97" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D97" s="2"/>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B98" t="s">
         <v>5</v>
       </c>
       <c r="C98" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D98" s="2"/>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B99" t="s">
         <v>5</v>
       </c>
       <c r="C99" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D99" s="2"/>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B100" t="s">
         <v>5</v>
       </c>
       <c r="C100" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D100" s="2"/>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B101" t="s">
         <v>5</v>
       </c>
       <c r="C101" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D101" s="2"/>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B102" t="s">
         <v>5</v>
       </c>
       <c r="C102" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D102" s="2"/>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B103" t="s">
         <v>5</v>
       </c>
       <c r="C103" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D103" s="2"/>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B104" t="s">
         <v>5</v>
       </c>
       <c r="C104" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D104" s="2"/>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B105" t="s">
         <v>5</v>
       </c>
       <c r="C105" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D105" s="2"/>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B106" t="s">
         <v>5</v>
       </c>
       <c r="C106" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D106" s="2"/>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B107" t="s">
         <v>5</v>
       </c>
       <c r="C107" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D107" s="2"/>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B108" t="s">
         <v>5</v>
       </c>
       <c r="C108" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D108" s="2"/>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B109" t="s">
         <v>5</v>
       </c>
       <c r="C109" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D109" s="2"/>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B110" t="s">
         <v>5</v>
       </c>
       <c r="C110" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D110" s="2"/>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B111" t="s">
         <v>5</v>
       </c>
       <c r="C111" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D111" s="2"/>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B112" t="s">
         <v>5</v>
       </c>
       <c r="C112" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D112" s="2"/>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B113" t="s">
         <v>5</v>
       </c>
       <c r="C113" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D113" s="2"/>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B114" t="s">
         <v>5</v>
       </c>
       <c r="C114" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D114" s="2"/>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B115" t="s">
         <v>5</v>
       </c>
       <c r="C115" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D115" s="2"/>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B116" t="s">
         <v>5</v>
       </c>
       <c r="C116" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D116" s="2"/>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B117" t="s">
         <v>5</v>
       </c>
       <c r="C117" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D117" s="2"/>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B118" t="s">
         <v>5</v>
       </c>
       <c r="C118" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D118" s="2"/>
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B119" t="s">
         <v>5</v>
       </c>
       <c r="C119" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D119" s="2"/>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B120" t="s">
         <v>5</v>
       </c>
       <c r="C120" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D120" s="2"/>
     </row>
     <row r="121">
       <c r="A121" t="s">
+        <v>278</v>
+      </c>
+      <c r="B121" t="s">
+        <v>279</v>
+      </c>
+      <c r="C121" t="s">
         <v>280</v>
-      </c>
-      <c r="B121" t="s">
-        <v>281</v>
-      </c>
-      <c r="C121" t="s">
-        <v>282</v>
       </c>
       <c r="D121" s="2"/>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B122" t="s">
         <v>5</v>
       </c>
       <c r="C122" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D122" s="2"/>
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B123" t="s">
         <v>5</v>
       </c>
       <c r="C123" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D123" s="2"/>
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B124" t="s">
         <v>5</v>
       </c>
       <c r="C124" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D124" s="2"/>
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B125" t="s">
         <v>5</v>
       </c>
       <c r="C125" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D125" s="2"/>
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B126" t="s">
         <v>5</v>
       </c>
       <c r="C126" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D126" s="2"/>
     </row>
     <row r="127">
       <c r="A127" t="s">
+        <v>290</v>
+      </c>
+      <c r="B127" t="s">
+        <v>291</v>
+      </c>
+      <c r="C127" t="s">
         <v>292</v>
-      </c>
-      <c r="B127" t="s">
-        <v>293</v>
-      </c>
-      <c r="C127" t="s">
-        <v>294</v>
       </c>
       <c r="D127" s="2"/>
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B128" t="s">
         <v>5</v>
       </c>
       <c r="C128" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D128" s="2"/>
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B129" t="s">
         <v>5</v>
       </c>
       <c r="C129" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D129" s="2"/>
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B130" t="s">
         <v>5</v>
       </c>
       <c r="C130" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D130" s="2"/>
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B131" t="s">
         <v>5</v>
       </c>
       <c r="C131" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D131" s="2"/>
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B132" t="s">
         <v>5</v>
       </c>
       <c r="C132" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D132" s="2"/>
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B133" t="s">
         <v>5</v>
       </c>
       <c r="C133" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D133" s="2"/>
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B134" t="s">
         <v>5</v>
       </c>
       <c r="C134" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D134" s="2"/>
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B135" t="s">
         <v>5</v>
       </c>
       <c r="C135" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D135" s="2"/>
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B136" t="s">
         <v>5</v>
       </c>
       <c r="C136" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D136" s="2"/>
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B137" t="s">
         <v>5</v>
       </c>
       <c r="C137" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D137" s="2"/>
     </row>
     <row r="138">
       <c r="A138" t="s">
+        <v>313</v>
+      </c>
+      <c r="B138" t="s">
+        <v>314</v>
+      </c>
+      <c r="C138" t="s">
         <v>315</v>
-      </c>
-      <c r="B138" t="s">
-        <v>316</v>
-      </c>
-      <c r="C138" t="s">
-        <v>317</v>
       </c>
       <c r="D138" s="2"/>
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B139" t="s">
         <v>5</v>
       </c>
       <c r="C139" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D139" s="2"/>
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B140" t="s">
         <v>5</v>
       </c>
       <c r="C140" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D140" s="2"/>
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B141" t="s">
         <v>5</v>
       </c>
       <c r="C141" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D141" s="2"/>
     </row>
     <row r="142">
       <c r="A142" t="s">
+        <v>321</v>
+      </c>
+      <c r="B142" t="s">
+        <v>322</v>
+      </c>
+      <c r="C142" t="s">
         <v>323</v>
-      </c>
-      <c r="B142" t="s">
-        <v>324</v>
-      </c>
-      <c r="C142" t="s">
-        <v>325</v>
       </c>
       <c r="D142" s="2"/>
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B143" t="s">
         <v>5</v>
       </c>
       <c r="C143" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D143" s="2"/>
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B144" t="s">
         <v>5</v>
       </c>
       <c r="C144" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D144" s="2"/>
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B145" t="s">
         <v>5</v>
       </c>
       <c r="C145" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D145" s="2"/>
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B146" t="s">
         <v>5</v>
       </c>
       <c r="C146" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D146" s="2"/>
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B147" t="s">
         <v>5</v>
       </c>
       <c r="C147" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D147" s="2"/>
     </row>
     <row r="148">
       <c r="A148" t="s">
+        <v>334</v>
+      </c>
+      <c r="B148" t="s">
+        <v>335</v>
+      </c>
+      <c r="C148" t="s">
         <v>336</v>
-      </c>
-      <c r="B148" t="s">
-        <v>337</v>
-      </c>
-      <c r="C148" t="s">
-        <v>338</v>
       </c>
       <c r="D148" s="2"/>
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B149" t="s">
         <v>5</v>
       </c>
       <c r="C149" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D149" s="2"/>
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B150" t="s">
         <v>5</v>
       </c>
       <c r="C150" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D150" s="2"/>
     </row>
     <row r="151">
       <c r="A151" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B151" t="s">
         <v>5</v>
       </c>
       <c r="C151" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D151" s="2"/>
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B152" t="s">
         <v>5</v>
       </c>
       <c r="C152" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D152" s="2"/>
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B153" t="s">
         <v>5</v>
       </c>
       <c r="C153" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D153" s="2"/>
     </row>
     <row r="154">
       <c r="A154" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B154" t="s">
         <v>5</v>
       </c>
       <c r="C154" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D154" s="2"/>
     </row>
     <row r="155">
       <c r="A155" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B155" t="s">
         <v>5</v>
       </c>
       <c r="C155" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D155" s="2"/>
     </row>
     <row r="156">
       <c r="A156" t="s">
+        <v>350</v>
+      </c>
+      <c r="B156" t="s">
+        <v>351</v>
+      </c>
+      <c r="C156" t="s">
         <v>352</v>
-      </c>
-      <c r="B156" t="s">
-        <v>353</v>
-      </c>
-      <c r="C156" t="s">
-        <v>354</v>
       </c>
       <c r="D156" s="2"/>
     </row>
     <row r="157">
       <c r="A157" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B157" t="s">
         <v>5</v>
       </c>
       <c r="C157" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D157" s="2"/>
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B158" t="s">
         <v>5</v>
       </c>
       <c r="C158" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D158" s="2"/>
     </row>
     <row r="159">
       <c r="A159" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B159" t="s">
         <v>5</v>
       </c>
       <c r="C159" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D159" s="2"/>
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B160" t="s">
         <v>5</v>
       </c>
       <c r="C160" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D160" s="2"/>
     </row>
     <row r="161">
       <c r="A161" t="s">
+        <v>361</v>
+      </c>
+      <c r="B161" t="s">
+        <v>362</v>
+      </c>
+      <c r="C161" t="s">
         <v>363</v>
-      </c>
-      <c r="B161" t="s">
-        <v>364</v>
-      </c>
-      <c r="C161" t="s">
-        <v>365</v>
       </c>
       <c r="D161" s="2"/>
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B162" t="s">
         <v>5</v>
       </c>
       <c r="C162" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="D162" s="2"/>
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B163" t="s">
         <v>5</v>
       </c>
       <c r="C163" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D163" s="2"/>
     </row>
     <row r="164">
       <c r="A164" t="s">
+        <v>368</v>
+      </c>
+      <c r="B164" t="s">
+        <v>369</v>
+      </c>
+      <c r="C164" t="s">
         <v>370</v>
-      </c>
-      <c r="B164" t="s">
-        <v>371</v>
-      </c>
-      <c r="C164" t="s">
-        <v>372</v>
       </c>
       <c r="D164" s="2"/>
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B165" t="s">
         <v>5</v>
@@ -3613,673 +3599,673 @@
     </row>
     <row r="166">
       <c r="A166" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B166" t="s">
         <v>5</v>
       </c>
       <c r="C166" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D166" s="2"/>
     </row>
     <row r="167">
       <c r="A167" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B167" t="s">
         <v>5</v>
       </c>
       <c r="C167" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D167" s="2"/>
     </row>
     <row r="168">
       <c r="A168" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B168" t="s">
         <v>5</v>
       </c>
       <c r="C168" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D168" s="2"/>
     </row>
     <row r="169">
       <c r="A169" t="s">
+        <v>378</v>
+      </c>
+      <c r="B169" t="s">
+        <v>379</v>
+      </c>
+      <c r="C169" t="s">
         <v>380</v>
-      </c>
-      <c r="B169" t="s">
-        <v>381</v>
-      </c>
-      <c r="C169" t="s">
-        <v>382</v>
       </c>
       <c r="D169" s="2"/>
     </row>
     <row r="170">
       <c r="A170" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B170" t="s">
         <v>5</v>
       </c>
       <c r="C170" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D170" s="2"/>
     </row>
     <row r="171">
       <c r="A171" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B171" t="s">
         <v>5</v>
       </c>
       <c r="C171" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D171" s="2"/>
     </row>
     <row r="172">
       <c r="A172" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B172" t="s">
         <v>5</v>
       </c>
       <c r="C172" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D172" s="2"/>
     </row>
     <row r="173">
       <c r="A173" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B173" t="s">
         <v>5</v>
       </c>
       <c r="C173" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D173" s="2"/>
     </row>
     <row r="174">
       <c r="A174" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B174" t="s">
         <v>5</v>
       </c>
       <c r="C174" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D174" s="2"/>
     </row>
     <row r="175">
       <c r="A175" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B175" t="s">
         <v>5</v>
       </c>
       <c r="C175" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D175" s="2"/>
     </row>
     <row r="176">
       <c r="A176" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B176" t="s">
         <v>5</v>
       </c>
       <c r="C176" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D176" s="2"/>
     </row>
     <row r="177">
       <c r="A177" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B177" t="s">
         <v>5</v>
       </c>
       <c r="C177" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D177" s="2"/>
     </row>
     <row r="178">
       <c r="A178" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B178" t="s">
         <v>5</v>
       </c>
       <c r="C178" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D178" s="2"/>
     </row>
     <row r="179">
       <c r="A179" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B179" t="s">
         <v>5</v>
       </c>
       <c r="C179" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D179" s="2"/>
     </row>
     <row r="180">
       <c r="A180" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B180" t="s">
         <v>5</v>
       </c>
       <c r="C180" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D180" s="2"/>
     </row>
     <row r="181">
       <c r="A181" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B181" t="s">
         <v>5</v>
       </c>
       <c r="C181" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D181" s="2"/>
     </row>
     <row r="182">
       <c r="A182" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B182" t="s">
         <v>5</v>
       </c>
       <c r="C182" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D182" s="2"/>
     </row>
     <row r="183">
       <c r="A183" t="s">
+        <v>407</v>
+      </c>
+      <c r="B183" t="s">
+        <v>408</v>
+      </c>
+      <c r="C183" t="s">
         <v>409</v>
-      </c>
-      <c r="B183" t="s">
-        <v>410</v>
-      </c>
-      <c r="C183" t="s">
-        <v>411</v>
       </c>
       <c r="D183" s="2"/>
     </row>
     <row r="184">
       <c r="A184" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B184" t="s">
         <v>5</v>
       </c>
       <c r="C184" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D184" s="2"/>
     </row>
     <row r="185">
       <c r="A185" t="s">
+        <v>412</v>
+      </c>
+      <c r="B185" t="s">
+        <v>413</v>
+      </c>
+      <c r="C185" t="s">
         <v>414</v>
-      </c>
-      <c r="B185" t="s">
-        <v>415</v>
-      </c>
-      <c r="C185" t="s">
-        <v>416</v>
       </c>
       <c r="D185" s="2"/>
     </row>
     <row r="186">
       <c r="A186" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B186" t="s">
         <v>5</v>
       </c>
       <c r="C186" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D186" s="2"/>
     </row>
     <row r="187">
       <c r="A187" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B187" t="s">
         <v>5</v>
       </c>
       <c r="C187" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D187" s="2"/>
     </row>
     <row r="188">
       <c r="A188" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B188" t="s">
         <v>5</v>
       </c>
       <c r="C188" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D188" s="2"/>
     </row>
     <row r="189">
       <c r="A189" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B189" t="s">
         <v>5</v>
       </c>
       <c r="C189" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D189" s="2"/>
     </row>
     <row r="190">
       <c r="A190" t="s">
+        <v>422</v>
+      </c>
+      <c r="B190" t="s">
+        <v>423</v>
+      </c>
+      <c r="C190" t="s">
         <v>424</v>
-      </c>
-      <c r="B190" t="s">
-        <v>425</v>
-      </c>
-      <c r="C190" t="s">
-        <v>426</v>
       </c>
       <c r="D190" s="2"/>
     </row>
     <row r="191">
       <c r="A191" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B191" t="s">
         <v>5</v>
       </c>
       <c r="C191" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D191" s="2"/>
     </row>
     <row r="192">
       <c r="A192" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B192" t="s">
         <v>5</v>
       </c>
       <c r="C192" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D192" s="2"/>
     </row>
     <row r="193">
       <c r="A193" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B193" t="s">
         <v>5</v>
       </c>
       <c r="C193" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D193" s="2"/>
     </row>
     <row r="194">
       <c r="A194" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B194" t="s">
         <v>5</v>
       </c>
       <c r="C194" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="D194" s="2"/>
     </row>
     <row r="195">
       <c r="A195" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B195" t="s">
         <v>5</v>
       </c>
       <c r="C195" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D195" s="2"/>
     </row>
     <row r="196">
       <c r="A196" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B196" t="s">
         <v>5</v>
       </c>
       <c r="C196" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D196" s="2"/>
     </row>
     <row r="197">
       <c r="A197" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B197" t="s">
         <v>5</v>
       </c>
       <c r="C197" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D197" s="2"/>
     </row>
     <row r="198">
       <c r="A198" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B198" t="s">
         <v>5</v>
       </c>
       <c r="C198" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D198" s="2"/>
     </row>
     <row r="199">
       <c r="A199" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B199" t="s">
         <v>5</v>
       </c>
       <c r="C199" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D199" s="2"/>
     </row>
     <row r="200">
       <c r="A200" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B200" t="s">
         <v>5</v>
       </c>
       <c r="C200" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D200" s="2"/>
     </row>
     <row r="201">
       <c r="A201" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B201" t="s">
         <v>5</v>
       </c>
       <c r="C201" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D201" s="2"/>
     </row>
     <row r="202">
       <c r="A202" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B202" t="s">
         <v>5</v>
       </c>
       <c r="C202" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D202" s="2"/>
     </row>
     <row r="203">
       <c r="A203" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B203" t="s">
         <v>5</v>
       </c>
       <c r="C203" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D203" s="2"/>
     </row>
     <row r="204">
       <c r="A204" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B204" t="s">
         <v>5</v>
       </c>
       <c r="C204" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D204" s="2"/>
     </row>
     <row r="205">
       <c r="A205" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B205" t="s">
         <v>5</v>
       </c>
       <c r="C205" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D205" s="2"/>
     </row>
     <row r="206">
       <c r="A206" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B206" t="s">
         <v>5</v>
       </c>
       <c r="C206" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D206" s="2"/>
     </row>
     <row r="207">
       <c r="A207" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B207" t="s">
         <v>5</v>
       </c>
       <c r="C207" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D207" s="2"/>
     </row>
     <row r="208">
       <c r="A208" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B208" t="s">
         <v>5</v>
       </c>
       <c r="C208" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D208" s="2"/>
     </row>
     <row r="209">
       <c r="A209" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B209" t="s">
         <v>5</v>
       </c>
       <c r="C209" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D209" s="2"/>
     </row>
     <row r="210">
       <c r="A210" t="s">
+        <v>460</v>
+      </c>
+      <c r="B210" t="s">
+        <v>461</v>
+      </c>
+      <c r="C210" t="s">
         <v>462</v>
-      </c>
-      <c r="B210" t="s">
-        <v>463</v>
-      </c>
-      <c r="C210" t="s">
-        <v>464</v>
       </c>
       <c r="D210" s="2"/>
     </row>
     <row r="211">
       <c r="A211" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B211" t="s">
         <v>5</v>
       </c>
       <c r="C211" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D211" s="2"/>
     </row>
     <row r="212">
       <c r="A212" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B212" t="s">
         <v>5</v>
       </c>
       <c r="C212" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D212" s="2"/>
     </row>
     <row r="213">
       <c r="A213" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B213" t="s">
         <v>5</v>
       </c>
       <c r="C213" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D213" s="2"/>
     </row>
     <row r="214">
       <c r="A214" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B214" t="s">
         <v>5</v>
       </c>
       <c r="C214" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D214" s="2"/>
     </row>
     <row r="215">
       <c r="A215" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B215" t="s">
         <v>5</v>
       </c>
       <c r="C215" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D215" s="2"/>
     </row>
     <row r="216">
       <c r="A216" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B216" t="s">
         <v>5</v>
       </c>
       <c r="C216" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D216" s="2"/>
     </row>
     <row r="217">
       <c r="A217" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B217" t="s">
         <v>5</v>
       </c>
       <c r="C217" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D217" s="2"/>
     </row>
     <row r="218">
       <c r="A218" t="s">
+        <v>477</v>
+      </c>
+      <c r="B218" t="s">
+        <v>478</v>
+      </c>
+      <c r="C218" t="s">
         <v>479</v>
-      </c>
-      <c r="B218" t="s">
-        <v>480</v>
-      </c>
-      <c r="C218" t="s">
-        <v>481</v>
       </c>
       <c r="D218" s="2"/>
     </row>
     <row r="219">
       <c r="A219" t="s">
+        <v>480</v>
+      </c>
+      <c r="B219" t="s">
+        <v>481</v>
+      </c>
+      <c r="C219" t="s">
         <v>482</v>
-      </c>
-      <c r="B219" t="s">
-        <v>483</v>
-      </c>
-      <c r="C219" t="s">
-        <v>484</v>
       </c>
       <c r="D219" s="2"/>
     </row>
     <row r="220">
       <c r="A220" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B220" t="s">
         <v>5</v>
       </c>
       <c r="C220" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D220" s="2"/>
     </row>
     <row r="221">
       <c r="A221" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="B221" t="s">
         <v>5</v>
       </c>
       <c r="C221" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D221" s="2"/>
     </row>

</xml_diff>